<commit_message>
fixed some errors from last update
</commit_message>
<xml_diff>
--- a/resources/NoteAudit.xlsx
+++ b/resources/NoteAudit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="1229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="1228">
   <si>
     <t>Name</t>
   </si>
@@ -3697,9 +3697,6 @@
   </si>
   <si>
     <t>(//button[@aria-label="Order Audit" and @ng-click="vm.go(entry.state)"])</t>
-  </si>
-  <si>
-    <t>Firstname</t>
   </si>
   <si>
     <t>(//button[@class="_md-no-style md-button md-cs-content-theme-theme md-ink-ripple"])[1]</t>
@@ -4063,8 +4060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J776"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4250,7 +4247,7 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>1227</v>
+        <v>12</v>
       </c>
       <c r="J7" t="s">
         <v>100</v>
@@ -16728,7 +16725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -16930,7 +16927,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Note audit - Treatment planning & education fix
</commit_message>
<xml_diff>
--- a/resources/NoteAudit.xlsx
+++ b/resources/NoteAudit.xlsx
@@ -3315,9 +3315,6 @@
     <t>Performed teach back method</t>
   </si>
   <si>
-    <t>//md-radio-group[@ng-model="vm.charts.education.understanding.detail"]//md-radio-button[@aria-checked="true" and @aria-label="Low (&lt; 50%)"]</t>
-  </si>
-  <si>
     <t>//md-radio-group[@ng-model="vm.charts.education.teachback.detail"]//md-radio-button[@aria-checked="true" and @aria-label="Low (&lt; 50%)"]</t>
   </si>
   <si>
@@ -3774,7 +3771,10 @@
     <t>//md-checkbox[@ng-model="vm.charts.careCoordination.conference.displinaryTeam" and @aria-checked="true"]</t>
   </si>
   <si>
-    <t>(//md-slider[@ng-model="vm.charts.vital[sign.name].bloodPressure.systolicBp" and @aria-valuenow="89"])[1]</t>
+    <t>(//md-slider[@ng-model="vm.charts.vital[sign.name].bloodPressure.systolicBp" and @aria-valuenow="90"])[1]</t>
+  </si>
+  <si>
+    <t>//md-select[@ng-model="vm.charts.education.teachingTool" and @aria-label="Tool: Teach back technique"]</t>
   </si>
 </sst>
 </file>
@@ -4135,8 +4135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J797"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="B790" workbookViewId="0">
+      <selection activeCell="B799" sqref="B799"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4385,7 +4385,7 @@
         <v>39</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4">
@@ -4403,7 +4403,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -4423,7 +4423,7 @@
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
@@ -4443,7 +4443,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
@@ -5236,7 +5236,7 @@
         <v>101</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C51" t="s">
         <v>29</v>
@@ -5256,7 +5256,7 @@
         <v>102</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C52" t="s">
         <v>29</v>
@@ -5757,7 +5757,7 @@
         <v>142</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C79" t="s">
         <v>29</v>
@@ -5833,7 +5833,7 @@
         <v>148</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C84" t="s">
         <v>29</v>
@@ -11031,7 +11031,7 @@
     </row>
     <row r="412" spans="1:7" ht="30">
       <c r="B412" s="3" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C412" t="s">
         <v>29</v>
@@ -15317,7 +15317,7 @@
         <v>1073</v>
       </c>
       <c r="B686" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C686" t="s">
         <v>29</v>
@@ -15331,7 +15331,7 @@
     </row>
     <row r="687" spans="1:7">
       <c r="B687" s="3" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C687" t="s">
         <v>29</v>
@@ -15345,7 +15345,7 @@
     </row>
     <row r="688" spans="1:7">
       <c r="B688" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="C688" t="s">
         <v>39</v>
@@ -15362,10 +15362,10 @@
     </row>
     <row r="689" spans="1:7">
       <c r="A689" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B689" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C689" t="s">
         <v>29</v>
@@ -15379,10 +15379,10 @@
     </row>
     <row r="690" spans="1:7">
       <c r="A690" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B690" s="3" t="s">
         <v>1197</v>
-      </c>
-      <c r="B690" s="3" t="s">
-        <v>1198</v>
       </c>
       <c r="C690" t="s">
         <v>29</v>
@@ -15399,7 +15399,7 @@
         <v>1074</v>
       </c>
       <c r="B691" s="3" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C691" t="s">
         <v>29</v>
@@ -15413,7 +15413,7 @@
     </row>
     <row r="692" spans="1:7">
       <c r="B692" s="3" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C692" t="s">
         <v>29</v>
@@ -15427,7 +15427,7 @@
     </row>
     <row r="693" spans="1:7">
       <c r="B693" s="3" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="C693" t="s">
         <v>39</v>
@@ -15444,10 +15444,10 @@
     </row>
     <row r="694" spans="1:7">
       <c r="A694" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B694" s="3" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C694" t="s">
         <v>29</v>
@@ -15461,10 +15461,10 @@
     </row>
     <row r="695" spans="1:7">
       <c r="A695" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B695" s="3" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C695" t="s">
         <v>29</v>
@@ -15478,7 +15478,7 @@
     </row>
     <row r="696" spans="1:7">
       <c r="B696" s="3" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C696" t="s">
         <v>39</v>
@@ -15495,7 +15495,7 @@
     </row>
     <row r="697" spans="1:7">
       <c r="B697" s="3" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C697" t="s">
         <v>39</v>
@@ -15512,10 +15512,10 @@
     </row>
     <row r="698" spans="1:7">
       <c r="A698" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B698" s="3" t="s">
         <v>1206</v>
-      </c>
-      <c r="B698" s="3" t="s">
-        <v>1207</v>
       </c>
       <c r="C698" t="s">
         <v>29</v>
@@ -15529,7 +15529,7 @@
     </row>
     <row r="699" spans="1:7">
       <c r="B699" s="3" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C699" t="s">
         <v>29</v>
@@ -15543,7 +15543,7 @@
     </row>
     <row r="700" spans="1:7">
       <c r="B700" s="3" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C700" t="s">
         <v>29</v>
@@ -15557,7 +15557,7 @@
     </row>
     <row r="701" spans="1:7">
       <c r="B701" s="3" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="C701" t="s">
         <v>29</v>
@@ -15571,7 +15571,7 @@
     </row>
     <row r="702" spans="1:7">
       <c r="B702" s="3" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C702" t="s">
         <v>29</v>
@@ -15585,7 +15585,7 @@
     </row>
     <row r="703" spans="1:7">
       <c r="B703" s="3" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="C703" t="s">
         <v>29</v>
@@ -15599,7 +15599,7 @@
     </row>
     <row r="704" spans="1:7">
       <c r="B704" s="3" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="C704" t="s">
         <v>39</v>
@@ -15616,7 +15616,7 @@
     </row>
     <row r="705" spans="1:7">
       <c r="B705" s="3" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="C705" t="s">
         <v>29</v>
@@ -15630,7 +15630,7 @@
     </row>
     <row r="706" spans="1:7">
       <c r="B706" s="3" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="C706" t="s">
         <v>29</v>
@@ -15644,7 +15644,7 @@
     </row>
     <row r="707" spans="1:7">
       <c r="B707" s="3" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C707" t="s">
         <v>29</v>
@@ -15658,7 +15658,7 @@
     </row>
     <row r="708" spans="1:7">
       <c r="B708" s="3" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="C708" t="s">
         <v>29</v>
@@ -15672,7 +15672,7 @@
     </row>
     <row r="709" spans="1:7">
       <c r="B709" s="3" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="C709" t="s">
         <v>29</v>
@@ -15686,7 +15686,7 @@
     </row>
     <row r="710" spans="1:7">
       <c r="B710" s="3" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="C710" t="s">
         <v>29</v>
@@ -15700,7 +15700,7 @@
     </row>
     <row r="711" spans="1:7">
       <c r="B711" s="3" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="C711" t="s">
         <v>29</v>
@@ -15714,7 +15714,7 @@
     </row>
     <row r="712" spans="1:7">
       <c r="B712" s="3" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C712" t="s">
         <v>29</v>
@@ -15728,7 +15728,7 @@
     </row>
     <row r="713" spans="1:7">
       <c r="B713" s="3" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C713" t="s">
         <v>29</v>
@@ -15742,7 +15742,7 @@
     </row>
     <row r="714" spans="1:7">
       <c r="B714" s="3" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="C714" t="s">
         <v>29</v>
@@ -15756,7 +15756,7 @@
     </row>
     <row r="715" spans="1:7">
       <c r="B715" s="3" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C715" t="s">
         <v>29</v>
@@ -15770,7 +15770,7 @@
     </row>
     <row r="716" spans="1:7">
       <c r="B716" s="3" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C716" t="s">
         <v>29</v>
@@ -15784,7 +15784,7 @@
     </row>
     <row r="717" spans="1:7">
       <c r="B717" s="3" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="C717" t="s">
         <v>29</v>
@@ -15798,7 +15798,7 @@
     </row>
     <row r="718" spans="1:7">
       <c r="B718" s="3" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="C718" t="s">
         <v>29</v>
@@ -15846,7 +15846,7 @@
     </row>
     <row r="721" spans="1:7">
       <c r="B721" s="3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C721" t="s">
         <v>29</v>
@@ -15860,10 +15860,10 @@
     </row>
     <row r="722" spans="1:7">
       <c r="A722" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B722" s="3" t="s">
         <v>1229</v>
-      </c>
-      <c r="B722" s="3" t="s">
-        <v>1230</v>
       </c>
       <c r="C722" t="s">
         <v>29</v>
@@ -15894,10 +15894,10 @@
     </row>
     <row r="724" spans="1:7">
       <c r="A724" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B724" s="3" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="C724" t="s">
         <v>29</v>
@@ -15928,7 +15928,7 @@
     </row>
     <row r="726" spans="1:7">
       <c r="B726" s="3" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C726" t="s">
         <v>29</v>
@@ -15976,7 +15976,7 @@
     </row>
     <row r="729" spans="1:7">
       <c r="B729" s="3" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C729" t="s">
         <v>39</v>
@@ -15996,7 +15996,7 @@
         <v>1084</v>
       </c>
       <c r="B730" s="3" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C730" t="s">
         <v>29</v>
@@ -16010,7 +16010,7 @@
     </row>
     <row r="731" spans="1:7">
       <c r="B731" s="3" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C731" t="s">
         <v>29</v>
@@ -16024,7 +16024,7 @@
     </row>
     <row r="732" spans="1:7">
       <c r="B732" s="3" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C732" t="s">
         <v>29</v>
@@ -16038,7 +16038,7 @@
     </row>
     <row r="733" spans="1:7">
       <c r="B733" s="3" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C733" t="s">
         <v>29</v>
@@ -16052,7 +16052,7 @@
     </row>
     <row r="734" spans="1:7">
       <c r="B734" s="3" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C734" t="s">
         <v>39</v>
@@ -16069,7 +16069,7 @@
     </row>
     <row r="735" spans="1:7">
       <c r="A735" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B735" s="3" t="s">
         <v>1085</v>
@@ -16156,7 +16156,7 @@
     </row>
     <row r="741" spans="1:7">
       <c r="B741" s="3" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="C741" t="s">
         <v>39</v>
@@ -16173,10 +16173,10 @@
     </row>
     <row r="742" spans="1:7">
       <c r="A742" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B742" s="3" t="s">
         <v>1242</v>
-      </c>
-      <c r="B742" s="3" t="s">
-        <v>1243</v>
       </c>
       <c r="C742" t="s">
         <v>39</v>
@@ -16193,7 +16193,7 @@
     </row>
     <row r="743" spans="1:7">
       <c r="B743" s="3" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C743" t="s">
         <v>29</v>
@@ -16207,10 +16207,10 @@
     </row>
     <row r="744" spans="1:7">
       <c r="A744" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B744" s="3" t="s">
         <v>1245</v>
-      </c>
-      <c r="B744" s="3" t="s">
-        <v>1246</v>
       </c>
       <c r="C744" t="s">
         <v>39</v>
@@ -16227,7 +16227,7 @@
     </row>
     <row r="745" spans="1:7">
       <c r="B745" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="C745" t="s">
         <v>29</v>
@@ -16241,7 +16241,7 @@
     </row>
     <row r="746" spans="1:7">
       <c r="B746" s="3" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="C746" t="s">
         <v>39</v>
@@ -16286,7 +16286,7 @@
     </row>
     <row r="749" spans="1:7">
       <c r="B749" s="3" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="C749" t="s">
         <v>39</v>
@@ -16371,7 +16371,7 @@
     </row>
     <row r="754" spans="1:7">
       <c r="B754" s="3" t="s">
-        <v>1099</v>
+        <v>1252</v>
       </c>
       <c r="C754" t="s">
         <v>29</v>
@@ -16385,7 +16385,7 @@
     </row>
     <row r="755" spans="1:7">
       <c r="B755" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C755" t="s">
         <v>29</v>
@@ -16399,7 +16399,7 @@
     </row>
     <row r="756" spans="1:7">
       <c r="B756" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C756" t="s">
         <v>29</v>
@@ -16413,10 +16413,10 @@
     </row>
     <row r="757" spans="1:7">
       <c r="A757" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B757" s="3" t="s">
         <v>1102</v>
-      </c>
-      <c r="B757" s="3" t="s">
-        <v>1103</v>
       </c>
       <c r="C757" t="s">
         <v>39</v>
@@ -16433,7 +16433,7 @@
     </row>
     <row r="758" spans="1:7">
       <c r="B758" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C758" t="s">
         <v>39</v>
@@ -16450,7 +16450,7 @@
     </row>
     <row r="759" spans="1:7">
       <c r="B759" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C759" t="s">
         <v>29</v>
@@ -16464,10 +16464,10 @@
     </row>
     <row r="760" spans="1:7">
       <c r="A760" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B760" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C760" t="s">
         <v>29</v>
@@ -16481,10 +16481,10 @@
     </row>
     <row r="761" spans="1:7">
       <c r="A761" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B761" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C761" t="s">
         <v>29</v>
@@ -16498,10 +16498,10 @@
     </row>
     <row r="762" spans="1:7">
       <c r="A762" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B762" s="3" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="C762" t="s">
         <v>29</v>
@@ -16515,10 +16515,10 @@
     </row>
     <row r="763" spans="1:7">
       <c r="A763" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B763" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C763" t="s">
         <v>29</v>
@@ -16532,10 +16532,10 @@
     </row>
     <row r="764" spans="1:7">
       <c r="A764" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B764" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C764" t="s">
         <v>29</v>
@@ -16549,10 +16549,10 @@
     </row>
     <row r="765" spans="1:7">
       <c r="A765" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B765" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C765" t="s">
         <v>29</v>
@@ -16566,10 +16566,10 @@
     </row>
     <row r="766" spans="1:7">
       <c r="A766" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B766" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C766" t="s">
         <v>29</v>
@@ -16583,10 +16583,10 @@
     </row>
     <row r="767" spans="1:7" ht="30">
       <c r="A767" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B767" s="3" t="s">
         <v>1119</v>
-      </c>
-      <c r="B767" s="3" t="s">
-        <v>1120</v>
       </c>
       <c r="C767" t="s">
         <v>29</v>
@@ -16600,10 +16600,10 @@
     </row>
     <row r="768" spans="1:7">
       <c r="A768" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B768" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C768" t="s">
         <v>29</v>
@@ -16617,7 +16617,7 @@
     </row>
     <row r="769" spans="1:7">
       <c r="B769" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C769" t="s">
         <v>29</v>
@@ -16631,7 +16631,7 @@
     </row>
     <row r="770" spans="1:7">
       <c r="B770" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C770" t="s">
         <v>29</v>
@@ -16645,7 +16645,7 @@
     </row>
     <row r="771" spans="1:7">
       <c r="B771" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C771" t="s">
         <v>29</v>
@@ -16659,7 +16659,7 @@
     </row>
     <row r="772" spans="1:7" ht="30">
       <c r="B772" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C772" t="s">
         <v>29</v>
@@ -16673,10 +16673,10 @@
     </row>
     <row r="773" spans="1:7">
       <c r="A773" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B773" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C773" t="s">
         <v>29</v>
@@ -16690,10 +16690,10 @@
     </row>
     <row r="774" spans="1:7" ht="30">
       <c r="A774" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B774" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C774" t="s">
         <v>29</v>
@@ -16707,10 +16707,10 @@
     </row>
     <row r="775" spans="1:7" ht="30">
       <c r="A775" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B775" s="3" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C775" t="s">
         <v>29</v>
@@ -16724,10 +16724,10 @@
     </row>
     <row r="776" spans="1:7">
       <c r="A776" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B776" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="C776" t="s">
         <v>29</v>
@@ -16741,10 +16741,10 @@
     </row>
     <row r="777" spans="1:7">
       <c r="A777" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B777" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C777" t="s">
         <v>29</v>
@@ -16758,10 +16758,10 @@
     </row>
     <row r="778" spans="1:7">
       <c r="A778" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B778" s="3" t="s">
         <v>1134</v>
-      </c>
-      <c r="B778" s="3" t="s">
-        <v>1135</v>
       </c>
       <c r="C778" t="s">
         <v>29</v>
@@ -16775,10 +16775,10 @@
     </row>
     <row r="779" spans="1:7">
       <c r="A779" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B779" s="3" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C779" t="s">
         <v>29</v>
@@ -16792,10 +16792,10 @@
     </row>
     <row r="780" spans="1:7">
       <c r="A780" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B780" s="3" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C780" t="s">
         <v>29</v>
@@ -16809,10 +16809,10 @@
     </row>
     <row r="781" spans="1:7">
       <c r="A781" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B781" s="3" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C781" t="s">
         <v>29</v>
@@ -16826,10 +16826,10 @@
     </row>
     <row r="782" spans="1:7">
       <c r="A782" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B782" s="3" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C782" t="s">
         <v>29</v>
@@ -16843,10 +16843,10 @@
     </row>
     <row r="783" spans="1:7">
       <c r="A783" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B783" s="3" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C783" t="s">
         <v>29</v>
@@ -16860,10 +16860,10 @@
     </row>
     <row r="784" spans="1:7">
       <c r="A784" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B784" s="3" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C784" t="s">
         <v>29</v>
@@ -16877,10 +16877,10 @@
     </row>
     <row r="785" spans="1:7">
       <c r="A785" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B785" s="3" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C785" t="s">
         <v>29</v>
@@ -16894,16 +16894,16 @@
     </row>
     <row r="786" spans="1:7">
       <c r="A786" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B786" s="3" t="s">
         <v>1150</v>
-      </c>
-      <c r="B786" s="3" t="s">
-        <v>1151</v>
       </c>
       <c r="C786" t="s">
         <v>39</v>
       </c>
       <c r="D786" s="6" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F786" s="4">
         <v>1</v>
@@ -16914,16 +16914,16 @@
     </row>
     <row r="787" spans="1:7">
       <c r="A787" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B787" s="3" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C787" t="s">
         <v>39</v>
       </c>
       <c r="D787" s="6" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F787" s="4">
         <v>1</v>
@@ -16934,16 +16934,16 @@
     </row>
     <row r="788" spans="1:7">
       <c r="A788" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B788" s="3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C788" t="s">
         <v>39</v>
       </c>
       <c r="D788" s="6" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="F788" s="4">
         <v>1</v>
@@ -16954,16 +16954,16 @@
     </row>
     <row r="789" spans="1:7">
       <c r="A789" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B789" s="3" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C789" t="s">
         <v>39</v>
       </c>
       <c r="D789" s="6" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="F789" s="4">
         <v>1</v>
@@ -16974,16 +16974,16 @@
     </row>
     <row r="790" spans="1:7">
       <c r="A790" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B790" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C790" t="s">
         <v>39</v>
       </c>
       <c r="D790" s="6" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F790" s="4">
         <v>1</v>
@@ -16994,16 +16994,16 @@
     </row>
     <row r="791" spans="1:7">
       <c r="A791" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B791" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C791" t="s">
         <v>39</v>
       </c>
       <c r="D791" s="6" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F791" s="4">
         <v>1</v>
@@ -17014,16 +17014,16 @@
     </row>
     <row r="792" spans="1:7">
       <c r="A792" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B792" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="C792" t="s">
         <v>39</v>
       </c>
       <c r="D792" s="6" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F792" s="4">
         <v>1</v>
@@ -17034,16 +17034,16 @@
     </row>
     <row r="793" spans="1:7">
       <c r="A793" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B793" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C793" t="s">
         <v>39</v>
       </c>
       <c r="D793" s="6" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="F793" s="4">
         <v>1</v>
@@ -17054,16 +17054,16 @@
     </row>
     <row r="794" spans="1:7">
       <c r="A794" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B794" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C794" t="s">
         <v>39</v>
       </c>
       <c r="D794" s="6" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="F794" s="4">
         <v>1</v>
@@ -17074,16 +17074,16 @@
     </row>
     <row r="795" spans="1:7">
       <c r="A795" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B795" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C795" t="s">
         <v>39</v>
       </c>
       <c r="D795" s="6" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F795" s="4">
         <v>1</v>
@@ -17094,16 +17094,16 @@
     </row>
     <row r="796" spans="1:7">
       <c r="A796" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B796" s="3" t="s">
         <v>1162</v>
-      </c>
-      <c r="B796" s="3" t="s">
-        <v>1163</v>
       </c>
       <c r="C796" t="s">
         <v>39</v>
       </c>
       <c r="D796" s="6" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F796" s="4">
         <v>1</v>
@@ -17114,16 +17114,16 @@
     </row>
     <row r="797" spans="1:7">
       <c r="A797" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B797" s="3" t="s">
         <v>1164</v>
-      </c>
-      <c r="B797" s="3" t="s">
-        <v>1165</v>
       </c>
       <c r="C797" t="s">
         <v>39</v>
       </c>
       <c r="D797" s="6" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F797" s="4">
         <v>1</v>
@@ -17272,7 +17272,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -17347,7 +17347,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
@@ -17368,10 +17368,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B9" t="s">
         <v>1181</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1182</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -17386,15 +17386,15 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B10" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C10" t="s">
         <v>433</v>
@@ -17412,33 +17412,33 @@
         <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B11" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C11" t="s">
         <v>433</v>
       </c>
       <c r="D11" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
         <v>1187</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>1188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
note audit xpath fix
</commit_message>
<xml_diff>
--- a/resources/NoteAudit.xlsx
+++ b/resources/NoteAudit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2265" uniqueCount="1253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2265" uniqueCount="1254">
   <si>
     <t>Name</t>
   </si>
@@ -3537,18 +3537,6 @@
     <t>//md-radio-group[@ng-model="vm.charts.homebound.value"]//md-radio-button[@aria-checked="true" and @aria-label="Yes"]</t>
   </si>
   <si>
-    <t>S43.129D: Disloc of unsp acromioclav jt, 100%-200% displacmnt, subs</t>
-  </si>
-  <si>
-    <t>S66.300A: Unsp inj extn musc/fasc/tend r idx fngr at wrs/hnd lv, init</t>
-  </si>
-  <si>
-    <t>S02.600B: Fx unsp part of body of mandible, unspecified side, 7thB</t>
-  </si>
-  <si>
-    <t>S36.400D: Unspecified injury of duodenum, subsequent encounter</t>
-  </si>
-  <si>
     <t>//md-slider[@ng-model="vm.charts.notifyphysician.temperature.lessThan" and @aria-valuenow="729"]</t>
   </si>
   <si>
@@ -3775,6 +3763,21 @@
   </si>
   <si>
     <t>//md-select[@ng-model="vm.charts.education.teachingTool" and @aria-label="Tool: Teach back technique"]</t>
+  </si>
+  <si>
+    <t>M75.100: Unspecified rotator cuff tear or rupture of unspecified shoulder, not specified as traumatic</t>
+  </si>
+  <si>
+    <t>M23.200: Derangement of unspecified lateral meniscus due to old tear or injury, right knee</t>
+  </si>
+  <si>
+    <t>S66.300A: Unspecified injury of extensor muscle, fascia and tendon of right index finger at wrist and hand level, initial encounter</t>
+  </si>
+  <si>
+    <t>S12.400K: Unspecified displaced fracture of fifth cervical vertebra, subsequent encounter for fracture with nonunion</t>
+  </si>
+  <si>
+    <t>S02.600G: Fracture of unspecified part of body of mandible, unspecified side, subsequent encounter for fracture with delayed healing</t>
   </si>
 </sst>
 </file>
@@ -4135,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J797"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B790" workbookViewId="0">
-      <selection activeCell="B799" sqref="B799"/>
+    <sheetView tabSelected="1" topLeftCell="A787" workbookViewId="0">
+      <selection activeCell="B794" sqref="B794"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4144,7 +4147,8 @@
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="151.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="122.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.28515625" customWidth="1"/>
@@ -5236,7 +5240,7 @@
         <v>101</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C51" t="s">
         <v>29</v>
@@ -5256,7 +5260,7 @@
         <v>102</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="C52" t="s">
         <v>29</v>
@@ -5757,7 +5761,7 @@
         <v>142</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="C79" t="s">
         <v>29</v>
@@ -11031,7 +11035,7 @@
     </row>
     <row r="412" spans="1:7" ht="30">
       <c r="B412" s="3" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="C412" t="s">
         <v>29</v>
@@ -15317,7 +15321,7 @@
         <v>1073</v>
       </c>
       <c r="B686" s="3" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="C686" t="s">
         <v>29</v>
@@ -15331,7 +15335,7 @@
     </row>
     <row r="687" spans="1:7">
       <c r="B687" s="3" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="C687" t="s">
         <v>29</v>
@@ -15345,7 +15349,7 @@
     </row>
     <row r="688" spans="1:7">
       <c r="B688" s="3" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="C688" t="s">
         <v>39</v>
@@ -15362,10 +15366,10 @@
     </row>
     <row r="689" spans="1:7">
       <c r="A689" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="B689" s="3" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="C689" t="s">
         <v>29</v>
@@ -15379,10 +15383,10 @@
     </row>
     <row r="690" spans="1:7">
       <c r="A690" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="B690" s="3" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="C690" t="s">
         <v>29</v>
@@ -15399,7 +15403,7 @@
         <v>1074</v>
       </c>
       <c r="B691" s="3" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="C691" t="s">
         <v>29</v>
@@ -15413,7 +15417,7 @@
     </row>
     <row r="692" spans="1:7">
       <c r="B692" s="3" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="C692" t="s">
         <v>29</v>
@@ -15427,7 +15431,7 @@
     </row>
     <row r="693" spans="1:7">
       <c r="B693" s="3" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="C693" t="s">
         <v>39</v>
@@ -15444,10 +15448,10 @@
     </row>
     <row r="694" spans="1:7">
       <c r="A694" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="B694" s="3" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="C694" t="s">
         <v>29</v>
@@ -15461,10 +15465,10 @@
     </row>
     <row r="695" spans="1:7">
       <c r="A695" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="B695" s="3" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="C695" t="s">
         <v>29</v>
@@ -15478,7 +15482,7 @@
     </row>
     <row r="696" spans="1:7">
       <c r="B696" s="3" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="C696" t="s">
         <v>39</v>
@@ -15495,7 +15499,7 @@
     </row>
     <row r="697" spans="1:7">
       <c r="B697" s="3" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="C697" t="s">
         <v>39</v>
@@ -15512,10 +15516,10 @@
     </row>
     <row r="698" spans="1:7">
       <c r="A698" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="B698" s="3" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="C698" t="s">
         <v>29</v>
@@ -15529,7 +15533,7 @@
     </row>
     <row r="699" spans="1:7">
       <c r="B699" s="3" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="C699" t="s">
         <v>29</v>
@@ -15543,7 +15547,7 @@
     </row>
     <row r="700" spans="1:7">
       <c r="B700" s="3" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="C700" t="s">
         <v>29</v>
@@ -15557,7 +15561,7 @@
     </row>
     <row r="701" spans="1:7">
       <c r="B701" s="3" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="C701" t="s">
         <v>29</v>
@@ -15571,7 +15575,7 @@
     </row>
     <row r="702" spans="1:7">
       <c r="B702" s="3" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="C702" t="s">
         <v>29</v>
@@ -15585,7 +15589,7 @@
     </row>
     <row r="703" spans="1:7">
       <c r="B703" s="3" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="C703" t="s">
         <v>29</v>
@@ -15599,7 +15603,7 @@
     </row>
     <row r="704" spans="1:7">
       <c r="B704" s="3" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="C704" t="s">
         <v>39</v>
@@ -15616,7 +15620,7 @@
     </row>
     <row r="705" spans="1:7">
       <c r="B705" s="3" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="C705" t="s">
         <v>29</v>
@@ -15630,7 +15634,7 @@
     </row>
     <row r="706" spans="1:7">
       <c r="B706" s="3" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="C706" t="s">
         <v>29</v>
@@ -15644,7 +15648,7 @@
     </row>
     <row r="707" spans="1:7">
       <c r="B707" s="3" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="C707" t="s">
         <v>29</v>
@@ -15658,7 +15662,7 @@
     </row>
     <row r="708" spans="1:7">
       <c r="B708" s="3" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C708" t="s">
         <v>29</v>
@@ -15672,7 +15676,7 @@
     </row>
     <row r="709" spans="1:7">
       <c r="B709" s="3" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="C709" t="s">
         <v>29</v>
@@ -15686,7 +15690,7 @@
     </row>
     <row r="710" spans="1:7">
       <c r="B710" s="3" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="C710" t="s">
         <v>29</v>
@@ -15700,7 +15704,7 @@
     </row>
     <row r="711" spans="1:7">
       <c r="B711" s="3" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="C711" t="s">
         <v>29</v>
@@ -15714,7 +15718,7 @@
     </row>
     <row r="712" spans="1:7">
       <c r="B712" s="3" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="C712" t="s">
         <v>29</v>
@@ -15728,7 +15732,7 @@
     </row>
     <row r="713" spans="1:7">
       <c r="B713" s="3" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="C713" t="s">
         <v>29</v>
@@ -15742,7 +15746,7 @@
     </row>
     <row r="714" spans="1:7">
       <c r="B714" s="3" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="C714" t="s">
         <v>29</v>
@@ -15756,7 +15760,7 @@
     </row>
     <row r="715" spans="1:7">
       <c r="B715" s="3" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="C715" t="s">
         <v>29</v>
@@ -15770,7 +15774,7 @@
     </row>
     <row r="716" spans="1:7">
       <c r="B716" s="3" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="C716" t="s">
         <v>29</v>
@@ -15784,7 +15788,7 @@
     </row>
     <row r="717" spans="1:7">
       <c r="B717" s="3" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="C717" t="s">
         <v>29</v>
@@ -15798,7 +15802,7 @@
     </row>
     <row r="718" spans="1:7">
       <c r="B718" s="3" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="C718" t="s">
         <v>29</v>
@@ -15846,7 +15850,7 @@
     </row>
     <row r="721" spans="1:7">
       <c r="B721" s="3" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="C721" t="s">
         <v>29</v>
@@ -15860,10 +15864,10 @@
     </row>
     <row r="722" spans="1:7">
       <c r="A722" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="B722" s="3" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="C722" t="s">
         <v>29</v>
@@ -15894,10 +15898,10 @@
     </row>
     <row r="724" spans="1:7">
       <c r="A724" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="B724" s="3" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="C724" t="s">
         <v>29</v>
@@ -15928,7 +15932,7 @@
     </row>
     <row r="726" spans="1:7">
       <c r="B726" s="3" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="C726" t="s">
         <v>29</v>
@@ -15976,7 +15980,7 @@
     </row>
     <row r="729" spans="1:7">
       <c r="B729" s="3" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="C729" t="s">
         <v>39</v>
@@ -15996,7 +16000,7 @@
         <v>1084</v>
       </c>
       <c r="B730" s="3" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="C730" t="s">
         <v>29</v>
@@ -16010,7 +16014,7 @@
     </row>
     <row r="731" spans="1:7">
       <c r="B731" s="3" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="C731" t="s">
         <v>29</v>
@@ -16024,7 +16028,7 @@
     </row>
     <row r="732" spans="1:7">
       <c r="B732" s="3" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="C732" t="s">
         <v>29</v>
@@ -16038,7 +16042,7 @@
     </row>
     <row r="733" spans="1:7">
       <c r="B733" s="3" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="C733" t="s">
         <v>29</v>
@@ -16052,7 +16056,7 @@
     </row>
     <row r="734" spans="1:7">
       <c r="B734" s="3" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="C734" t="s">
         <v>39</v>
@@ -16069,7 +16073,7 @@
     </row>
     <row r="735" spans="1:7">
       <c r="A735" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="B735" s="3" t="s">
         <v>1085</v>
@@ -16156,7 +16160,7 @@
     </row>
     <row r="741" spans="1:7">
       <c r="B741" s="3" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="C741" t="s">
         <v>39</v>
@@ -16173,10 +16177,10 @@
     </row>
     <row r="742" spans="1:7">
       <c r="A742" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B742" s="3" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="C742" t="s">
         <v>39</v>
@@ -16193,7 +16197,7 @@
     </row>
     <row r="743" spans="1:7">
       <c r="B743" s="3" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="C743" t="s">
         <v>29</v>
@@ -16207,10 +16211,10 @@
     </row>
     <row r="744" spans="1:7">
       <c r="A744" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="B744" s="3" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="C744" t="s">
         <v>39</v>
@@ -16227,7 +16231,7 @@
     </row>
     <row r="745" spans="1:7">
       <c r="B745" s="3" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="C745" t="s">
         <v>29</v>
@@ -16241,7 +16245,7 @@
     </row>
     <row r="746" spans="1:7">
       <c r="B746" s="3" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="C746" t="s">
         <v>39</v>
@@ -16286,7 +16290,7 @@
     </row>
     <row r="749" spans="1:7">
       <c r="B749" s="3" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="C749" t="s">
         <v>39</v>
@@ -16371,7 +16375,7 @@
     </row>
     <row r="754" spans="1:7">
       <c r="B754" s="3" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="C754" t="s">
         <v>29</v>
@@ -16501,7 +16505,7 @@
         <v>1109</v>
       </c>
       <c r="B762" s="3" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="C762" t="s">
         <v>29</v>
@@ -16903,7 +16907,7 @@
         <v>39</v>
       </c>
       <c r="D786" s="6" t="s">
-        <v>1173</v>
+        <v>1249</v>
       </c>
       <c r="F786" s="4">
         <v>1</v>
@@ -16923,7 +16927,7 @@
         <v>39</v>
       </c>
       <c r="D787" s="6" t="s">
-        <v>1173</v>
+        <v>1250</v>
       </c>
       <c r="F787" s="4">
         <v>1</v>
@@ -16943,7 +16947,7 @@
         <v>39</v>
       </c>
       <c r="D788" s="6" t="s">
-        <v>1174</v>
+        <v>1251</v>
       </c>
       <c r="F788" s="4">
         <v>1</v>
@@ -16963,7 +16967,7 @@
         <v>39</v>
       </c>
       <c r="D789" s="6" t="s">
-        <v>1176</v>
+        <v>1252</v>
       </c>
       <c r="F789" s="4">
         <v>1</v>
@@ -16983,7 +16987,7 @@
         <v>39</v>
       </c>
       <c r="D790" s="6" t="s">
-        <v>1175</v>
+        <v>1253</v>
       </c>
       <c r="F790" s="4">
         <v>1</v>
@@ -17003,7 +17007,7 @@
         <v>39</v>
       </c>
       <c r="D791" s="6" t="s">
-        <v>1173</v>
+        <v>1249</v>
       </c>
       <c r="F791" s="4">
         <v>1</v>
@@ -17023,7 +17027,7 @@
         <v>39</v>
       </c>
       <c r="D792" s="6" t="s">
-        <v>1173</v>
+        <v>1250</v>
       </c>
       <c r="F792" s="4">
         <v>1</v>
@@ -17043,7 +17047,7 @@
         <v>39</v>
       </c>
       <c r="D793" s="6" t="s">
-        <v>1174</v>
+        <v>1251</v>
       </c>
       <c r="F793" s="4">
         <v>1</v>
@@ -17063,7 +17067,7 @@
         <v>39</v>
       </c>
       <c r="D794" s="6" t="s">
-        <v>1176</v>
+        <v>1252</v>
       </c>
       <c r="F794" s="4">
         <v>1</v>
@@ -17083,7 +17087,7 @@
         <v>39</v>
       </c>
       <c r="D795" s="6" t="s">
-        <v>1175</v>
+        <v>1253</v>
       </c>
       <c r="F795" s="4">
         <v>1</v>
@@ -17103,7 +17107,7 @@
         <v>39</v>
       </c>
       <c r="D796" s="6" t="s">
-        <v>1173</v>
+        <v>1249</v>
       </c>
       <c r="F796" s="4">
         <v>1</v>
@@ -17123,7 +17127,7 @@
         <v>39</v>
       </c>
       <c r="D797" s="6" t="s">
-        <v>1173</v>
+        <v>1249</v>
       </c>
       <c r="F797" s="4">
         <v>1</v>
@@ -17272,7 +17276,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -17347,7 +17351,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
@@ -17368,10 +17372,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="B9" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -17386,15 +17390,15 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="B10" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="C10" t="s">
         <v>433</v>
@@ -17412,21 +17416,21 @@
         <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="B11" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="C11" t="s">
         <v>433</v>
       </c>
       <c r="D11" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -17438,7 +17442,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>